<commit_message>
created BOM list of components from farnell
</commit_message>
<xml_diff>
--- a/purchase/components.xlsx
+++ b/purchase/components.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t xml:space="preserve">Part Number</t>
   </si>
@@ -31,13 +31,13 @@
     <t xml:space="preserve">Line Note</t>
   </si>
   <si>
-    <t xml:space="preserve">hlavni spinac</t>
+    <t xml:space="preserve">Main switch (waterproof)</t>
   </si>
   <si>
     <t xml:space="preserve">R13-112F8-02-BB-2A</t>
   </si>
   <si>
-    <t xml:space="preserve">indikator nabiti</t>
+    <t xml:space="preserve">Charging indicator</t>
   </si>
   <si>
     <t xml:space="preserve">3v3 LDO</t>
@@ -46,94 +46,238 @@
     <t xml:space="preserve">XC6220B331MR-G</t>
   </si>
   <si>
-    <t xml:space="preserve">5V LDO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MC7805CD2TR4G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">idealni dioda</t>
+    <t xml:space="preserve">5V DC/DC converter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TPS62140RGTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ideal Diode</t>
   </si>
   <si>
     <t xml:space="preserve">MAX40200AUK+T</t>
   </si>
   <si>
-    <t xml:space="preserve">bateriovy manager</t>
+    <t xml:space="preserve">BMS chip</t>
   </si>
   <si>
     <t xml:space="preserve">LTC2943IDD#TRPBF</t>
   </si>
   <si>
-    <t xml:space="preserve">vykonovy p channel mosfet</t>
+    <t xml:space="preserve">Voltage detector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APX803L-40W5-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">555 casovac THT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LM555CN/NOPB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buzzer 12V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABI-010-RC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schottky diode SOD 123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBR0520</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current fuses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MP005472</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DPS socket, CLIK-Mate 3 pin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">502494-0370</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DPS socket, CLIK-Mate 4 pin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">502494-0470</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DPS socket, CLIK-Mate 8 pin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">502494-0870</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DPS connector, CLIK-Mate 3 pin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">502439-0300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DPS connector, CLIK-Mate 4 pin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">502439-0400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DPS connector, CLIK-Mate 8 pin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">502439-0800</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contacts CLIK-Mate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">502438-0000</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">2.2uH </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">inductor for DC/DC converter</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">DFE252012P-2R2M=P2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Transistor SMD </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">BC847</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">BC847C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P-Channel MOSFET</t>
   </si>
   <si>
     <t xml:space="preserve">SIS415DNT-T1-GE3</t>
   </si>
   <si>
-    <t xml:space="preserve">spi flash pamet 8-SOIC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S25FL064LABMFI010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">odpor pro snimani proudu 0.002 1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MPR123WF200NT4E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">resistor 1k 805 1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CRGCQ0805J1K0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">resistor 4k7 805 5%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AC0805JR-074K7L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">resistor 10k 805</t>
+    <t xml:space="preserve">Resistor 0R 805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MC0805S8F0000T5E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current sense resistor 0.01 2512 1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PE2512FKE070R01L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistor 200 805 5%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0805FR-07200RL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistor 2k7 805 1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0805FR-072K7L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistor 5k1 805 5%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0805JR-075K1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistor 10k 805</t>
   </si>
   <si>
     <t xml:space="preserve">CRCW080510K0FKEC</t>
   </si>
   <si>
-    <t xml:space="preserve">resistor 200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0805FR-07200RL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kondenzator 0.1uF 10% 805</t>
+    <t xml:space="preserve">Resistor 100k 805 5%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0805JR-10100KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistor 590k 805 1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0805FR-07590KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacitor 680pF 10% 805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC0805KRX7R9BB681</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacitor 0.1uF 10% 805</t>
   </si>
   <si>
     <t xml:space="preserve">CL21B104KBCNNND</t>
   </si>
   <si>
-    <t xml:space="preserve">kodenzator 0.33 uF 10% 805</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CL21B334KBFNNNE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">senzor proudu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INA219AIDCNR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kondenzator 10uF 10% 805</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CL21A106KOQNNNF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kondenzator 4.7uF 10% 805</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CL21A475KOFNNNG</t>
+    <t xml:space="preserve">Capacitor 220nF 10% 805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRM21AR72A224KAC5K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacitor 1uF 10% 805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CL21B105KAFNNNE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacitor 10 uF 10% 805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRM21BC80J106KE19L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacitor 22uF 10 % 805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRM21BC80J226ME51L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacitor 47uF 10% 805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CL21A476MQCLRNC</t>
   </si>
 </sst>
 </file>
@@ -143,7 +287,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -188,19 +332,38 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="0"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBFBFBF"/>
-        <bgColor rgb="FFCCCCFF"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -237,7 +400,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -250,15 +413,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -271,66 +450,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFBFBFBF"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -514,14 +633,14 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="32.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="41.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="32.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="5" style="1" width="8.43"/>
   </cols>
@@ -564,13 +683,13 @@
       <c r="A2" s="1" t="n">
         <v>1634656</v>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B2" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="0" t="s">
         <v>4</v>
       </c>
     </row>
@@ -578,13 +697,13 @@
       <c r="A3" s="1" t="n">
         <v>3932127</v>
       </c>
-      <c r="B3" s="4" t="n">
+      <c r="B3" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="5" t="n">
+      <c r="D3" s="4" t="n">
         <v>104020006</v>
       </c>
     </row>
@@ -592,27 +711,27 @@
       <c r="A4" s="1" t="n">
         <v>1830935</v>
       </c>
-      <c r="B4" s="4" t="n">
+      <c r="B4" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
-        <v>1652337</v>
-      </c>
-      <c r="B5" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="C5" s="4" t="s">
+        <v>3007429</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -620,13 +739,13 @@
       <c r="A6" s="1" t="n">
         <v>3404609</v>
       </c>
-      <c r="B6" s="4" t="n">
+      <c r="B6" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -634,228 +753,790 @@
       <c r="A7" s="1" t="n">
         <v>4027957</v>
       </c>
-      <c r="B7" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="B7" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
-        <v>3772839</v>
-      </c>
-      <c r="B8" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="C8" s="4" t="s">
+        <v>3589297</v>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
-        <v>2768034</v>
-      </c>
-      <c r="B9" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C9" s="4" t="s">
+        <v>3121177</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
-        <v>4227473</v>
-      </c>
-      <c r="B10" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="A10" s="0" t="n">
+        <v>1022399</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="0" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
-        <v>2861907</v>
-      </c>
-      <c r="B11" s="4" t="n">
-        <v>100</v>
-      </c>
-      <c r="C11" s="4" t="s">
+        <v>2533224</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
-        <v>3495339</v>
-      </c>
-      <c r="B12" s="4" t="n">
-        <v>100</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="A12" s="0" t="n">
+        <v>3564732</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C12" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="0" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
-        <v>4139748</v>
-      </c>
-      <c r="B13" s="4" t="n">
-        <v>100</v>
-      </c>
-      <c r="C13" s="4" t="s">
+        <v>2914017</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
-        <v>3495998</v>
-      </c>
-      <c r="B14" s="4" t="n">
-        <v>100</v>
-      </c>
-      <c r="C14" s="4" t="s">
+        <v>1617068</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
-        <v>4539029</v>
-      </c>
-      <c r="B15" s="4" t="n">
-        <v>100</v>
-      </c>
-      <c r="C15" s="4" t="s">
+        <v>3221826</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
-        <v>4539154</v>
-      </c>
-      <c r="B16" s="4" t="n">
-        <v>100</v>
-      </c>
-      <c r="C16" s="4" t="s">
+        <v>2913997</v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
-        <v>3118164</v>
-      </c>
-      <c r="B17" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C17" s="4" t="s">
+        <v>1617057</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
-        <v>4539078</v>
-      </c>
-      <c r="B18" s="4" t="n">
-        <v>100</v>
-      </c>
-      <c r="C18" s="4" t="s">
+        <v>3864009</v>
+      </c>
+      <c r="B18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
-        <v>4539118</v>
-      </c>
-      <c r="B19" s="4" t="n">
-        <v>100</v>
-      </c>
-      <c r="C19" s="4" t="s">
+        <v>2313700</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="n">
+        <v>2530074</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="n">
+        <v>4553395</v>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="n">
+        <v>3772839</v>
+      </c>
+      <c r="B22" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="n">
+        <v>2309112</v>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="n">
+        <v>3951690</v>
+      </c>
+      <c r="B24" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="n">
+        <v>3495998</v>
+      </c>
+      <c r="B25" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="n">
+        <v>9237666</v>
+      </c>
+      <c r="B26" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="n">
+        <v>3496134</v>
+      </c>
+      <c r="B27" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="n">
+        <v>4139748</v>
+      </c>
+      <c r="B28" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="n">
+        <v>4013422</v>
+      </c>
+      <c r="B29" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="n">
+        <v>3952338</v>
+      </c>
+      <c r="B30" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="n">
+        <v>3019860</v>
+      </c>
+      <c r="B31" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="n">
+        <v>4539029</v>
+      </c>
+      <c r="B32" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="9" t="n">
+        <v>3785973</v>
+      </c>
+      <c r="B33" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="n">
+        <v>3013481</v>
+      </c>
+      <c r="B34" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="n">
+        <v>4327048</v>
+      </c>
+      <c r="B35" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="n">
+        <v>4361089</v>
+      </c>
+      <c r="B36" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="n">
+        <v>3013465</v>
+      </c>
+      <c r="B37" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0"/>
+      <c r="B38" s="0"/>
+      <c r="C38" s="0"/>
+      <c r="D38" s="0"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0"/>
+      <c r="B39" s="0"/>
+      <c r="C39" s="0"/>
+      <c r="D39" s="0"/>
+      <c r="E39" s="0"/>
+      <c r="F39" s="0"/>
+      <c r="G39" s="0"/>
+      <c r="H39" s="0"/>
+      <c r="I39" s="0"/>
+      <c r="J39" s="0"/>
+      <c r="K39" s="0"/>
+      <c r="L39" s="0"/>
+      <c r="M39" s="0"/>
+      <c r="N39" s="0"/>
+      <c r="O39" s="0"/>
+      <c r="P39" s="0"/>
+      <c r="Q39" s="0"/>
+      <c r="R39" s="0"/>
+      <c r="S39" s="0"/>
+      <c r="T39" s="0"/>
+      <c r="U39" s="0"/>
+      <c r="V39" s="0"/>
+      <c r="W39" s="0"/>
+      <c r="X39" s="0"/>
+      <c r="Y39" s="0"/>
+      <c r="Z39" s="0"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0"/>
+      <c r="B40" s="0"/>
+      <c r="C40" s="0"/>
+      <c r="D40" s="0"/>
+      <c r="E40" s="0"/>
+      <c r="F40" s="0"/>
+      <c r="G40" s="0"/>
+      <c r="H40" s="0"/>
+      <c r="I40" s="0"/>
+      <c r="J40" s="0"/>
+      <c r="K40" s="0"/>
+      <c r="L40" s="0"/>
+      <c r="M40" s="0"/>
+      <c r="N40" s="0"/>
+      <c r="O40" s="0"/>
+      <c r="P40" s="0"/>
+      <c r="Q40" s="0"/>
+      <c r="R40" s="0"/>
+      <c r="S40" s="0"/>
+      <c r="T40" s="0"/>
+      <c r="U40" s="0"/>
+      <c r="V40" s="0"/>
+      <c r="W40" s="0"/>
+      <c r="X40" s="0"/>
+      <c r="Y40" s="0"/>
+      <c r="Z40" s="0"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0"/>
+      <c r="B41" s="0"/>
+      <c r="C41" s="0"/>
+      <c r="D41" s="0"/>
+      <c r="E41" s="0"/>
+      <c r="F41" s="0"/>
+      <c r="G41" s="0"/>
+      <c r="H41" s="0"/>
+      <c r="I41" s="0"/>
+      <c r="J41" s="0"/>
+      <c r="K41" s="0"/>
+      <c r="L41" s="0"/>
+      <c r="M41" s="0"/>
+      <c r="N41" s="0"/>
+      <c r="O41" s="0"/>
+      <c r="P41" s="0"/>
+      <c r="Q41" s="0"/>
+      <c r="R41" s="0"/>
+      <c r="S41" s="0"/>
+      <c r="T41" s="0"/>
+      <c r="U41" s="0"/>
+      <c r="V41" s="0"/>
+      <c r="W41" s="0"/>
+      <c r="X41" s="0"/>
+      <c r="Y41" s="0"/>
+      <c r="Z41" s="0"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0"/>
+      <c r="B42" s="0"/>
+      <c r="C42" s="0"/>
+      <c r="D42" s="0"/>
+      <c r="E42" s="0"/>
+      <c r="F42" s="0"/>
+      <c r="G42" s="0"/>
+      <c r="H42" s="0"/>
+      <c r="I42" s="0"/>
+      <c r="J42" s="0"/>
+      <c r="K42" s="0"/>
+      <c r="L42" s="0"/>
+      <c r="M42" s="0"/>
+      <c r="N42" s="0"/>
+      <c r="O42" s="0"/>
+      <c r="P42" s="0"/>
+      <c r="Q42" s="0"/>
+      <c r="R42" s="0"/>
+      <c r="S42" s="0"/>
+      <c r="T42" s="0"/>
+      <c r="U42" s="0"/>
+      <c r="V42" s="0"/>
+      <c r="W42" s="0"/>
+      <c r="X42" s="0"/>
+      <c r="Y42" s="0"/>
+      <c r="Z42" s="0"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0"/>
+      <c r="B43" s="0"/>
+      <c r="C43" s="0"/>
+      <c r="D43" s="0"/>
+      <c r="E43" s="0"/>
+      <c r="F43" s="0"/>
+      <c r="G43" s="0"/>
+      <c r="H43" s="0"/>
+      <c r="I43" s="0"/>
+      <c r="J43" s="0"/>
+      <c r="K43" s="0"/>
+      <c r="L43" s="0"/>
+      <c r="M43" s="0"/>
+      <c r="N43" s="0"/>
+      <c r="O43" s="0"/>
+      <c r="P43" s="0"/>
+      <c r="Q43" s="0"/>
+      <c r="R43" s="0"/>
+      <c r="S43" s="0"/>
+      <c r="T43" s="0"/>
+      <c r="U43" s="0"/>
+      <c r="V43" s="0"/>
+      <c r="W43" s="0"/>
+      <c r="X43" s="0"/>
+      <c r="Y43" s="0"/>
+      <c r="Z43" s="0"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0"/>
+      <c r="B44" s="0"/>
+      <c r="C44" s="0"/>
+      <c r="D44" s="0"/>
+      <c r="E44" s="0"/>
+      <c r="F44" s="0"/>
+      <c r="G44" s="0"/>
+      <c r="H44" s="0"/>
+      <c r="I44" s="0"/>
+      <c r="J44" s="0"/>
+      <c r="K44" s="0"/>
+      <c r="L44" s="0"/>
+      <c r="M44" s="0"/>
+      <c r="N44" s="0"/>
+      <c r="O44" s="0"/>
+      <c r="P44" s="0"/>
+      <c r="Q44" s="0"/>
+      <c r="R44" s="0"/>
+      <c r="S44" s="0"/>
+      <c r="T44" s="0"/>
+      <c r="U44" s="0"/>
+      <c r="V44" s="0"/>
+      <c r="W44" s="0"/>
+      <c r="X44" s="0"/>
+      <c r="Y44" s="0"/>
+      <c r="Z44" s="0"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0"/>
+      <c r="B45" s="0"/>
+      <c r="C45" s="0"/>
+      <c r="D45" s="0"/>
+      <c r="E45" s="0"/>
+      <c r="F45" s="0"/>
+      <c r="G45" s="0"/>
+      <c r="H45" s="0"/>
+      <c r="I45" s="0"/>
+      <c r="J45" s="0"/>
+      <c r="K45" s="0"/>
+      <c r="L45" s="0"/>
+      <c r="M45" s="0"/>
+      <c r="N45" s="0"/>
+      <c r="O45" s="0"/>
+      <c r="P45" s="0"/>
+      <c r="Q45" s="0"/>
+      <c r="R45" s="0"/>
+      <c r="S45" s="0"/>
+      <c r="T45" s="0"/>
+      <c r="U45" s="0"/>
+      <c r="V45" s="0"/>
+      <c r="W45" s="0"/>
+      <c r="X45" s="0"/>
+      <c r="Y45" s="0"/>
+      <c r="Z45" s="0"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0"/>
+      <c r="B46" s="0"/>
+      <c r="C46" s="0"/>
+      <c r="D46" s="0"/>
+      <c r="E46" s="0"/>
+      <c r="F46" s="0"/>
+      <c r="G46" s="0"/>
+      <c r="H46" s="0"/>
+      <c r="I46" s="0"/>
+      <c r="J46" s="0"/>
+      <c r="K46" s="0"/>
+      <c r="L46" s="0"/>
+      <c r="M46" s="0"/>
+      <c r="N46" s="0"/>
+      <c r="O46" s="0"/>
+      <c r="P46" s="0"/>
+      <c r="Q46" s="0"/>
+      <c r="R46" s="0"/>
+      <c r="S46" s="0"/>
+      <c r="T46" s="0"/>
+      <c r="U46" s="0"/>
+      <c r="V46" s="0"/>
+      <c r="W46" s="0"/>
+      <c r="X46" s="0"/>
+      <c r="Y46" s="0"/>
+      <c r="Z46" s="0"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0"/>
+      <c r="B47" s="0"/>
+      <c r="C47" s="0"/>
+      <c r="D47" s="0"/>
+      <c r="E47" s="0"/>
+      <c r="F47" s="0"/>
+      <c r="G47" s="0"/>
+      <c r="H47" s="0"/>
+      <c r="I47" s="0"/>
+      <c r="J47" s="0"/>
+      <c r="K47" s="0"/>
+      <c r="L47" s="0"/>
+      <c r="M47" s="0"/>
+      <c r="N47" s="0"/>
+      <c r="O47" s="0"/>
+      <c r="P47" s="0"/>
+      <c r="Q47" s="0"/>
+      <c r="R47" s="0"/>
+      <c r="S47" s="0"/>
+      <c r="T47" s="0"/>
+      <c r="U47" s="0"/>
+      <c r="V47" s="0"/>
+      <c r="W47" s="0"/>
+      <c r="X47" s="0"/>
+      <c r="Y47" s="0"/>
+      <c r="Z47" s="0"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0"/>
+      <c r="B48" s="0"/>
+      <c r="C48" s="0"/>
+      <c r="D48" s="0"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0"/>
+      <c r="B49" s="0"/>
+      <c r="C49" s="0"/>
+      <c r="D49" s="0"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0"/>
+      <c r="B50" s="0"/>
+      <c r="C50" s="0"/>
+      <c r="D50" s="0"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0"/>
+      <c r="B51" s="0"/>
+      <c r="C51" s="0"/>
+      <c r="D51" s="0"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0"/>
+      <c r="B52" s="0"/>
+      <c r="C52" s="0"/>
+      <c r="D52" s="0"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0"/>
+      <c r="B53" s="0"/>
+      <c r="C53" s="0"/>
+      <c r="D53" s="0"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0"/>
+      <c r="B54" s="0"/>
+      <c r="C54" s="0"/>
+      <c r="D54" s="0"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0"/>
+      <c r="B55" s="0"/>
+      <c r="C55" s="0"/>
+      <c r="D55" s="0"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0"/>
+      <c r="B56" s="0"/>
+      <c r="C56" s="0"/>
+      <c r="D56" s="0"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0"/>
+      <c r="B57" s="0"/>
+      <c r="C57" s="0"/>
+      <c r="D57" s="0"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0"/>
+      <c r="B58" s="0"/>
+      <c r="C58" s="0"/>
+      <c r="D58" s="0"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0"/>
+      <c r="B59" s="0"/>
+      <c r="C59" s="0"/>
+      <c r="D59" s="0"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0"/>
+      <c r="B60" s="0"/>
+      <c r="C60" s="0"/>
+      <c r="D60" s="0"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0"/>
+      <c r="B61" s="0"/>
+      <c r="C61" s="0"/>
+      <c r="D61" s="0"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0"/>
+      <c r="B62" s="0"/>
+      <c r="C62" s="0"/>
+      <c r="D62" s="0"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0"/>
+      <c r="B63" s="0"/>
+      <c r="C63" s="0"/>
+      <c r="D63" s="0"/>
+    </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
components numbers adjusted to be able to manufacture 5 systems
</commit_message>
<xml_diff>
--- a/purchase/components.xlsx
+++ b/purchase/components.xlsx
@@ -136,49 +136,13 @@
     <t xml:space="preserve">502438-0000</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">2.2uH </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">inductor for DC/DC converter</t>
-    </r>
+    <t xml:space="preserve">2.2uH inductor for DC/DC converter</t>
   </si>
   <si>
     <t xml:space="preserve">DFE252012P-2R2M=P2</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Transistor SMD </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">BC847</t>
-    </r>
+    <t xml:space="preserve">Transistor SMD BC847</t>
   </si>
   <si>
     <t xml:space="preserve">BC847C</t>
@@ -287,7 +251,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -317,45 +281,6 @@
       <name val="Tahoma"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Tahoma"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Tahoma"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Tahoma"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -400,7 +325,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -410,34 +335,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -633,10 +530,10 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9"/>
@@ -683,13 +580,13 @@
       <c r="A2" s="1" t="n">
         <v>1634656</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="B2" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -697,13 +594,13 @@
       <c r="A3" s="1" t="n">
         <v>3932127</v>
       </c>
-      <c r="B3" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D3" s="4" t="n">
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="n">
         <v>104020006</v>
       </c>
     </row>
@@ -711,13 +608,13 @@
       <c r="A4" s="1" t="n">
         <v>1830935</v>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -725,13 +622,13 @@
       <c r="A5" s="1" t="n">
         <v>3007429</v>
       </c>
-      <c r="B5" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -739,13 +636,13 @@
       <c r="A6" s="1" t="n">
         <v>3404609</v>
       </c>
-      <c r="B6" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="B6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -753,13 +650,13 @@
       <c r="A7" s="1" t="n">
         <v>4027957</v>
       </c>
-      <c r="B7" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -767,13 +664,13 @@
       <c r="A8" s="1" t="n">
         <v>3589297</v>
       </c>
-      <c r="B8" s="3" t="n">
+      <c r="B8" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -782,9 +679,9 @@
         <v>3121177</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -792,16 +689,16 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>1022399</v>
       </c>
-      <c r="B10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" s="0" t="s">
+      <c r="B10" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -812,24 +709,24 @@
       <c r="B11" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <v>3564732</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -838,7 +735,7 @@
         <v>2914017</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>24</v>
@@ -852,9 +749,9 @@
         <v>1617068</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -866,9 +763,9 @@
         <v>3221826</v>
       </c>
       <c r="B15" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -880,9 +777,9 @@
         <v>2913997</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -894,9 +791,9 @@
         <v>1617057</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -908,9 +805,9 @@
         <v>3864009</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -922,7 +819,7 @@
         <v>2313700</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>36</v>
@@ -938,7 +835,7 @@
       <c r="B20" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -963,13 +860,13 @@
       <c r="A22" s="1" t="n">
         <v>3772839</v>
       </c>
-      <c r="B22" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C22" s="3" t="s">
+      <c r="B22" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="1" t="s">
         <v>43</v>
       </c>
     </row>
@@ -978,9 +875,9 @@
         <v>2309112</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="C23" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -994,7 +891,7 @@
       <c r="B24" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -1005,13 +902,13 @@
       <c r="A25" s="1" t="n">
         <v>3495998</v>
       </c>
-      <c r="B25" s="3" t="n">
+      <c r="B25" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="1" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1047,13 +944,13 @@
       <c r="A28" s="1" t="n">
         <v>4139748</v>
       </c>
-      <c r="B28" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="C28" s="3" t="s">
+      <c r="B28" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="1" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1064,7 +961,7 @@
       <c r="B29" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1078,7 +975,7 @@
       <c r="B30" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D30" s="1" t="s">
@@ -1092,7 +989,7 @@
       <c r="B31" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="1" t="s">
         <v>60</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -1103,27 +1000,27 @@
       <c r="A32" s="1" t="n">
         <v>4539029</v>
       </c>
-      <c r="B32" s="3" t="n">
+      <c r="B32" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="9" t="n">
+      <c r="A33" s="1" t="n">
         <v>3785973</v>
       </c>
       <c r="B33" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="D33" s="1" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1134,7 +1031,7 @@
       <c r="B34" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="C34" s="1" t="s">
         <v>66</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -1148,7 +1045,7 @@
       <c r="B35" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -1162,7 +1059,7 @@
       <c r="B36" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" s="1" t="s">
         <v>70</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -1176,367 +1073,39 @@
       <c r="B37" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C37" s="1" t="s">
         <v>72</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0"/>
-      <c r="B38" s="0"/>
-      <c r="C38" s="0"/>
-      <c r="D38" s="0"/>
-    </row>
-    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0"/>
-      <c r="B39" s="0"/>
-      <c r="C39" s="0"/>
-      <c r="D39" s="0"/>
-      <c r="E39" s="0"/>
-      <c r="F39" s="0"/>
-      <c r="G39" s="0"/>
-      <c r="H39" s="0"/>
-      <c r="I39" s="0"/>
-      <c r="J39" s="0"/>
-      <c r="K39" s="0"/>
-      <c r="L39" s="0"/>
-      <c r="M39" s="0"/>
-      <c r="N39" s="0"/>
-      <c r="O39" s="0"/>
-      <c r="P39" s="0"/>
-      <c r="Q39" s="0"/>
-      <c r="R39" s="0"/>
-      <c r="S39" s="0"/>
-      <c r="T39" s="0"/>
-      <c r="U39" s="0"/>
-      <c r="V39" s="0"/>
-      <c r="W39" s="0"/>
-      <c r="X39" s="0"/>
-      <c r="Y39" s="0"/>
-      <c r="Z39" s="0"/>
-    </row>
-    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0"/>
-      <c r="B40" s="0"/>
-      <c r="C40" s="0"/>
-      <c r="D40" s="0"/>
-      <c r="E40" s="0"/>
-      <c r="F40" s="0"/>
-      <c r="G40" s="0"/>
-      <c r="H40" s="0"/>
-      <c r="I40" s="0"/>
-      <c r="J40" s="0"/>
-      <c r="K40" s="0"/>
-      <c r="L40" s="0"/>
-      <c r="M40" s="0"/>
-      <c r="N40" s="0"/>
-      <c r="O40" s="0"/>
-      <c r="P40" s="0"/>
-      <c r="Q40" s="0"/>
-      <c r="R40" s="0"/>
-      <c r="S40" s="0"/>
-      <c r="T40" s="0"/>
-      <c r="U40" s="0"/>
-      <c r="V40" s="0"/>
-      <c r="W40" s="0"/>
-      <c r="X40" s="0"/>
-      <c r="Y40" s="0"/>
-      <c r="Z40" s="0"/>
-    </row>
-    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0"/>
-      <c r="B41" s="0"/>
-      <c r="C41" s="0"/>
-      <c r="D41" s="0"/>
-      <c r="E41" s="0"/>
-      <c r="F41" s="0"/>
-      <c r="G41" s="0"/>
-      <c r="H41" s="0"/>
-      <c r="I41" s="0"/>
-      <c r="J41" s="0"/>
-      <c r="K41" s="0"/>
-      <c r="L41" s="0"/>
-      <c r="M41" s="0"/>
-      <c r="N41" s="0"/>
-      <c r="O41" s="0"/>
-      <c r="P41" s="0"/>
-      <c r="Q41" s="0"/>
-      <c r="R41" s="0"/>
-      <c r="S41" s="0"/>
-      <c r="T41" s="0"/>
-      <c r="U41" s="0"/>
-      <c r="V41" s="0"/>
-      <c r="W41" s="0"/>
-      <c r="X41" s="0"/>
-      <c r="Y41" s="0"/>
-      <c r="Z41" s="0"/>
-    </row>
-    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0"/>
-      <c r="B42" s="0"/>
-      <c r="C42" s="0"/>
-      <c r="D42" s="0"/>
-      <c r="E42" s="0"/>
-      <c r="F42" s="0"/>
-      <c r="G42" s="0"/>
-      <c r="H42" s="0"/>
-      <c r="I42" s="0"/>
-      <c r="J42" s="0"/>
-      <c r="K42" s="0"/>
-      <c r="L42" s="0"/>
-      <c r="M42" s="0"/>
-      <c r="N42" s="0"/>
-      <c r="O42" s="0"/>
-      <c r="P42" s="0"/>
-      <c r="Q42" s="0"/>
-      <c r="R42" s="0"/>
-      <c r="S42" s="0"/>
-      <c r="T42" s="0"/>
-      <c r="U42" s="0"/>
-      <c r="V42" s="0"/>
-      <c r="W42" s="0"/>
-      <c r="X42" s="0"/>
-      <c r="Y42" s="0"/>
-      <c r="Z42" s="0"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0"/>
-      <c r="B43" s="0"/>
-      <c r="C43" s="0"/>
-      <c r="D43" s="0"/>
-      <c r="E43" s="0"/>
-      <c r="F43" s="0"/>
-      <c r="G43" s="0"/>
-      <c r="H43" s="0"/>
-      <c r="I43" s="0"/>
-      <c r="J43" s="0"/>
-      <c r="K43" s="0"/>
-      <c r="L43" s="0"/>
-      <c r="M43" s="0"/>
-      <c r="N43" s="0"/>
-      <c r="O43" s="0"/>
-      <c r="P43" s="0"/>
-      <c r="Q43" s="0"/>
-      <c r="R43" s="0"/>
-      <c r="S43" s="0"/>
-      <c r="T43" s="0"/>
-      <c r="U43" s="0"/>
-      <c r="V43" s="0"/>
-      <c r="W43" s="0"/>
-      <c r="X43" s="0"/>
-      <c r="Y43" s="0"/>
-      <c r="Z43" s="0"/>
-    </row>
-    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0"/>
-      <c r="B44" s="0"/>
-      <c r="C44" s="0"/>
-      <c r="D44" s="0"/>
-      <c r="E44" s="0"/>
-      <c r="F44" s="0"/>
-      <c r="G44" s="0"/>
-      <c r="H44" s="0"/>
-      <c r="I44" s="0"/>
-      <c r="J44" s="0"/>
-      <c r="K44" s="0"/>
-      <c r="L44" s="0"/>
-      <c r="M44" s="0"/>
-      <c r="N44" s="0"/>
-      <c r="O44" s="0"/>
-      <c r="P44" s="0"/>
-      <c r="Q44" s="0"/>
-      <c r="R44" s="0"/>
-      <c r="S44" s="0"/>
-      <c r="T44" s="0"/>
-      <c r="U44" s="0"/>
-      <c r="V44" s="0"/>
-      <c r="W44" s="0"/>
-      <c r="X44" s="0"/>
-      <c r="Y44" s="0"/>
-      <c r="Z44" s="0"/>
-    </row>
-    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0"/>
-      <c r="B45" s="0"/>
-      <c r="C45" s="0"/>
-      <c r="D45" s="0"/>
-      <c r="E45" s="0"/>
-      <c r="F45" s="0"/>
-      <c r="G45" s="0"/>
-      <c r="H45" s="0"/>
-      <c r="I45" s="0"/>
-      <c r="J45" s="0"/>
-      <c r="K45" s="0"/>
-      <c r="L45" s="0"/>
-      <c r="M45" s="0"/>
-      <c r="N45" s="0"/>
-      <c r="O45" s="0"/>
-      <c r="P45" s="0"/>
-      <c r="Q45" s="0"/>
-      <c r="R45" s="0"/>
-      <c r="S45" s="0"/>
-      <c r="T45" s="0"/>
-      <c r="U45" s="0"/>
-      <c r="V45" s="0"/>
-      <c r="W45" s="0"/>
-      <c r="X45" s="0"/>
-      <c r="Y45" s="0"/>
-      <c r="Z45" s="0"/>
-    </row>
-    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0"/>
-      <c r="B46" s="0"/>
-      <c r="C46" s="0"/>
-      <c r="D46" s="0"/>
-      <c r="E46" s="0"/>
-      <c r="F46" s="0"/>
-      <c r="G46" s="0"/>
-      <c r="H46" s="0"/>
-      <c r="I46" s="0"/>
-      <c r="J46" s="0"/>
-      <c r="K46" s="0"/>
-      <c r="L46" s="0"/>
-      <c r="M46" s="0"/>
-      <c r="N46" s="0"/>
-      <c r="O46" s="0"/>
-      <c r="P46" s="0"/>
-      <c r="Q46" s="0"/>
-      <c r="R46" s="0"/>
-      <c r="S46" s="0"/>
-      <c r="T46" s="0"/>
-      <c r="U46" s="0"/>
-      <c r="V46" s="0"/>
-      <c r="W46" s="0"/>
-      <c r="X46" s="0"/>
-      <c r="Y46" s="0"/>
-      <c r="Z46" s="0"/>
-    </row>
-    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0"/>
-      <c r="B47" s="0"/>
-      <c r="C47" s="0"/>
-      <c r="D47" s="0"/>
-      <c r="E47" s="0"/>
-      <c r="F47" s="0"/>
-      <c r="G47" s="0"/>
-      <c r="H47" s="0"/>
-      <c r="I47" s="0"/>
-      <c r="J47" s="0"/>
-      <c r="K47" s="0"/>
-      <c r="L47" s="0"/>
-      <c r="M47" s="0"/>
-      <c r="N47" s="0"/>
-      <c r="O47" s="0"/>
-      <c r="P47" s="0"/>
-      <c r="Q47" s="0"/>
-      <c r="R47" s="0"/>
-      <c r="S47" s="0"/>
-      <c r="T47" s="0"/>
-      <c r="U47" s="0"/>
-      <c r="V47" s="0"/>
-      <c r="W47" s="0"/>
-      <c r="X47" s="0"/>
-      <c r="Y47" s="0"/>
-      <c r="Z47" s="0"/>
-    </row>
-    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0"/>
-      <c r="B48" s="0"/>
-      <c r="C48" s="0"/>
-      <c r="D48" s="0"/>
-    </row>
-    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0"/>
-      <c r="B49" s="0"/>
-      <c r="C49" s="0"/>
-      <c r="D49" s="0"/>
-    </row>
-    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0"/>
-      <c r="B50" s="0"/>
-      <c r="C50" s="0"/>
-      <c r="D50" s="0"/>
-    </row>
-    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0"/>
-      <c r="B51" s="0"/>
-      <c r="C51" s="0"/>
-      <c r="D51" s="0"/>
-    </row>
-    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0"/>
-      <c r="B52" s="0"/>
-      <c r="C52" s="0"/>
-      <c r="D52" s="0"/>
-    </row>
-    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0"/>
-      <c r="B53" s="0"/>
-      <c r="C53" s="0"/>
-      <c r="D53" s="0"/>
-    </row>
-    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0"/>
-      <c r="B54" s="0"/>
-      <c r="C54" s="0"/>
-      <c r="D54" s="0"/>
-    </row>
-    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0"/>
-      <c r="B55" s="0"/>
-      <c r="C55" s="0"/>
-      <c r="D55" s="0"/>
-    </row>
-    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0"/>
-      <c r="B56" s="0"/>
-      <c r="C56" s="0"/>
-      <c r="D56" s="0"/>
-    </row>
-    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0"/>
-      <c r="B57" s="0"/>
-      <c r="C57" s="0"/>
-      <c r="D57" s="0"/>
-    </row>
-    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0"/>
-      <c r="B58" s="0"/>
-      <c r="C58" s="0"/>
-      <c r="D58" s="0"/>
-    </row>
-    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0"/>
-      <c r="B59" s="0"/>
-      <c r="C59" s="0"/>
-      <c r="D59" s="0"/>
-    </row>
-    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0"/>
-      <c r="B60" s="0"/>
-      <c r="C60" s="0"/>
-      <c r="D60" s="0"/>
-    </row>
-    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0"/>
-      <c r="B61" s="0"/>
-      <c r="C61" s="0"/>
-      <c r="D61" s="0"/>
-    </row>
-    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0"/>
-      <c r="B62" s="0"/>
-      <c r="C62" s="0"/>
-      <c r="D62" s="0"/>
-    </row>
-    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0"/>
-      <c r="B63" s="0"/>
-      <c r="C63" s="0"/>
-      <c r="D63" s="0"/>
-    </row>
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>